<commit_message>
Update field log for bottom depth
</commit_message>
<xml_diff>
--- a/Experiment_Cruise_Instrument_Radiometry_Field_Log.xlsx
+++ b/Experiment_Cruise_Instrument_Radiometry_Field_Log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daurin/Projects/HyperPACE/field_data/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daurin/GitRepos/HyperCP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0AE641-F26A-B749-B62A-F967AAC0535D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B585BEAA-F829-DE46-8D44-59EC0AF1D1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39760" yWindow="-8680" windowWidth="36880" windowHeight="17300" xr2:uid="{334D9F36-0597-1A47-89E0-CF51DBBDBDB1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Station</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>(not for pySAS when working properly, or if station number is in the name)</t>
+  </si>
+  <si>
+    <t>Bottom Depth</t>
   </si>
 </sst>
 </file>
@@ -150,7 +153,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -163,79 +166,8 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -262,40 +194,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -611,18 +522,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354C5F92-70E2-8E4F-AD02-49BF65479048}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2060" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.33203125" customWidth="1"/>
     <col min="2" max="2" width="33.83203125" customWidth="1"/>
-    <col min="3" max="3" width="32.1640625" customWidth="1"/>
+    <col min="3" max="3" width="31.5" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" customWidth="1"/>
     <col min="6" max="6" width="8.5" customWidth="1"/>
@@ -631,26 +542,28 @@
     <col min="9" max="9" width="8.5" customWidth="1"/>
     <col min="10" max="10" width="7.5" customWidth="1"/>
     <col min="11" max="11" width="10.1640625" customWidth="1"/>
-    <col min="12" max="12" width="65.33203125" customWidth="1"/>
+    <col min="12" max="12" width="9.83203125" customWidth="1"/>
+    <col min="13" max="13" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -662,23 +575,25 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="10"/>
+    <row r="3" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -691,86 +606,93 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:13" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:L3"/>
+    <mergeCell ref="A1:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update field log for solar disk
</commit_message>
<xml_diff>
--- a/Experiment_Cruise_Instrument_Radiometry_Field_Log.xlsx
+++ b/Experiment_Cruise_Instrument_Radiometry_Field_Log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daurin/GitRepos/HyperCP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DA4755-071B-8040-8542-FB465BEEDDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E79E7BC-D724-334B-A7B4-5CB0005057DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39760" yWindow="-8680" windowWidth="39880" windowHeight="17300" xr2:uid="{334D9F36-0597-1A47-89E0-CF51DBBDBDB1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>lat</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>(kts)</t>
+  </si>
+  <si>
+    <t>solar disk</t>
+  </si>
+  <si>
+    <t>(T/F)</t>
   </si>
 </sst>
 </file>
@@ -223,14 +229,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -546,11 +552,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354C5F92-70E2-8E4F-AD02-49BF65479048}">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2580" activePane="bottomLeft"/>
-      <selection activeCell="S1" sqref="S1"/>
+      <pane ySplit="2580"/>
+      <selection activeCell="Q7" sqref="Q7"/>
       <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -571,73 +577,76 @@
     <col min="13" max="13" width="6.1640625" customWidth="1"/>
     <col min="14" max="14" width="7.5" customWidth="1"/>
     <col min="15" max="15" width="15.1640625" customWidth="1"/>
-    <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="18" max="18" width="52.33203125" customWidth="1"/>
+    <col min="16" max="17" width="10" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
     </row>
-    <row r="2" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
+    <row r="2" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
+    <row r="3" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -654,8 +663,9 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -680,10 +690,10 @@
       <c r="H5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="5" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -705,13 +715,16 @@
         <v>20</v>
       </c>
       <c r="Q5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -761,15 +774,18 @@
         <v>11</v>
       </c>
       <c r="Q6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="S6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:R3"/>
+    <mergeCell ref="A1:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update field log template
</commit_message>
<xml_diff>
--- a/Experiment_Cruise_Instrument_Radiometry_Field_Log.xlsx
+++ b/Experiment_Cruise_Instrument_Radiometry_Field_Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daurin/GitRepos/HyperCP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E79E7BC-D724-334B-A7B4-5CB0005057DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD160CA-28CE-4A48-9596-DF73E7415C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39760" yWindow="-8680" windowWidth="39880" windowHeight="17300" xr2:uid="{334D9F36-0597-1A47-89E0-CF51DBBDBDB1}"/>
+    <workbookView xWindow="45760" yWindow="2000" windowWidth="34560" windowHeight="21560" xr2:uid="{334D9F36-0597-1A47-89E0-CF51DBBDBDB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>lat</t>
   </si>
@@ -44,27 +44,15 @@
     <t>lon</t>
   </si>
   <si>
-    <t>Experiment name (preferably something agreed upon for SeaBASS submission later), ship/platform name, operator name. Set-up notes: for pySAS, min/max azimuth settings, azimuth offset (usually 0, but confirm), height above water, ship hull color, etc.</t>
-  </si>
-  <si>
-    <t>(name agreed across sampling platforms)</t>
-  </si>
-  <si>
     <t>(UTC)</t>
   </si>
   <si>
-    <t>(UTC. Confirm all systms set to UTC)</t>
-  </si>
-  <si>
     <t>(deg; 3-4 decimals)</t>
   </si>
   <si>
     <t>(deg)</t>
   </si>
   <si>
-    <t>(above-water; only if set manually)</t>
-  </si>
-  <si>
     <t>(m/s)</t>
   </si>
   <si>
@@ -86,15 +74,9 @@
     <t>wind speed</t>
   </si>
   <si>
-    <t>(not for pySAS when working properly, or if station number is in the name)</t>
-  </si>
-  <si>
     <t>(psu)</t>
   </si>
   <si>
-    <t>sea surface temperature</t>
-  </si>
-  <si>
     <t>salinity</t>
   </si>
   <si>
@@ -107,9 +89,6 @@
     <t>comments</t>
   </si>
   <si>
-    <t>station</t>
-  </si>
-  <si>
     <t>raw filename</t>
   </si>
   <si>
@@ -138,6 +117,39 @@
   </si>
   <si>
     <t>(T/F)</t>
+  </si>
+  <si>
+    <t>(not req'd for autonomous systems)</t>
+  </si>
+  <si>
+    <t>(not req'd for autonomous systems or where relative solar-sensor azimuth provided)</t>
+  </si>
+  <si>
+    <t>(deg; not req'd for autonomous systems)</t>
+  </si>
+  <si>
+    <t>(preferably numeric; agreed across sampling platforms)</t>
+  </si>
+  <si>
+    <t>station/cast</t>
+  </si>
+  <si>
+    <t>sea surface temp</t>
+  </si>
+  <si>
+    <t>air temp</t>
+  </si>
+  <si>
+    <t>(deg; only req'd for TriOS RAMSES G1)</t>
+  </si>
+  <si>
+    <t>(UTC. Confirm ALL systms set to UTC)</t>
+  </si>
+  <si>
+    <t>(not req'd for autonomous systems when working properly, or if station number is in the name or ancillary SeaBASS file)</t>
+  </si>
+  <si>
+    <t>Experiment name (agreed upon for SeaBASS submission), Cruise name, ship/platform name, operator name. Set-up notes: height above water, ship hull color, etc., for autonomous systems include min/max azimuth settings, azimuth offset (usually 0, but confirm).</t>
   </si>
 </sst>
 </file>
@@ -256,9 +268,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -296,7 +308,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -402,7 +414,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -544,7 +556,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -552,38 +564,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354C5F92-70E2-8E4F-AD02-49BF65479048}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2580"/>
-      <selection activeCell="Q7" sqref="Q7"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
     <col min="2" max="2" width="33.83203125" customWidth="1"/>
-    <col min="3" max="3" width="31.5" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
     <col min="6" max="6" width="7.5" customWidth="1"/>
     <col min="7" max="7" width="13.1640625" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
     <col min="9" max="9" width="14.6640625" customWidth="1"/>
     <col min="10" max="10" width="14.83203125" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" customWidth="1"/>
     <col min="12" max="12" width="8.1640625" customWidth="1"/>
     <col min="13" max="13" width="6.1640625" customWidth="1"/>
     <col min="14" max="14" width="7.5" customWidth="1"/>
-    <col min="15" max="15" width="15.1640625" customWidth="1"/>
+    <col min="15" max="15" width="8.1640625" customWidth="1"/>
     <col min="16" max="17" width="10" customWidth="1"/>
-    <col min="19" max="19" width="52.33203125" customWidth="1"/>
+    <col min="18" max="18" width="13.5" customWidth="1"/>
+    <col min="19" max="19" width="8.33203125" customWidth="1"/>
+    <col min="20" max="20" width="52.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -603,8 +615,9 @@
       <c r="Q1" s="7"/>
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
     </row>
-    <row r="2" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -624,8 +637,9 @@
       <c r="Q2" s="7"/>
       <c r="R2" s="7"/>
       <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
     </row>
-    <row r="3" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -645,8 +659,9 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
     </row>
-    <row r="4" spans="1:19" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -664,19 +679,20 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:19" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>0</v>
@@ -685,107 +701,113 @@
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="H6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="N6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="Q6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T6" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="A1:T3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>